<commit_message>
GradeSheet for 1 to 10 Fixed nearly
</commit_message>
<xml_diff>
--- a/.github/subjects11_12.xlsx
+++ b/.github/subjects11_12.xlsx
@@ -5,17 +5,30 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amirl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sms\sms\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84199B16-53FE-45E0-842C-39ED2D93B0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E96AD87-B13A-421C-8D92-7329B71627AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="1965" windowWidth="15375" windowHeight="7785" xr2:uid="{67CA5FF5-4EDD-45D5-BDB3-D06F7EEFAA34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67CA5FF5-4EDD-45D5-BDB3-D06F7EEFAA34}"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1016,7 +1029,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,6 +1037,7 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1064,7 +1078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1590,7 +1604,7 @@
         <v>12</v>
       </c>
       <c r="K15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1631,7 +1645,7 @@
         <v>22</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>